<commit_message>
Sadia sister  is not study
</commit_message>
<xml_diff>
--- a/Routine.xlsx
+++ b/Routine.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
   <si>
     <t>Saturday</t>
   </si>
@@ -90,9 +90,6 @@
   </si>
   <si>
     <t>Riyad(9-10)</t>
-  </si>
-  <si>
-    <t>Sadia Sister</t>
   </si>
   <si>
     <t>Jannatul Math</t>
@@ -342,9 +339,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -352,9 +352,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,7 +635,7 @@
   <dimension ref="A2:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,34 +655,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="8" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="5"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="7"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="7"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="10"/>
     </row>
     <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
@@ -724,80 +721,78 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="E5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="10"/>
+      <c r="E6" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="13"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="3"/>
+      <c r="J6" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -805,14 +800,14 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -822,96 +817,92 @@
         <v>21</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" s="11"/>
+        <v>33</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="14"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="3"/>
+      <c r="J8" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="K8" s="3"/>
       <c r="L8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="F9" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="10"/>
+      <c r="G9" s="13"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="3"/>
+      <c r="J10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="K10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K10" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="L10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -923,12 +914,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="F9:G9"/>
     <mergeCell ref="H2:L3"/>
     <mergeCell ref="A2:B3"/>
     <mergeCell ref="C2:G3"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Students name colour change
</commit_message>
<xml_diff>
--- a/Routine.xlsx
+++ b/Routine.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
   <si>
     <t>Saturday</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>Jannatul(HSC)</t>
-  </si>
-  <si>
-    <t>Sormi</t>
   </si>
   <si>
     <t>Riyad(9-10)</t>
@@ -147,7 +144,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,6 +189,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -334,12 +338,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -349,9 +355,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,7 +640,7 @@
   <dimension ref="A2:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,34 +660,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="11" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="7"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="9"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="10"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="12"/>
     </row>
     <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
@@ -724,174 +729,174 @@
       <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="E5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="15" t="s">
         <v>23</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>20</v>
+      <c r="B6" s="15" t="s">
+        <v>19</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="13"/>
+      <c r="E6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="6"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3" t="s">
-        <v>25</v>
+      <c r="J6" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3" t="s">
+      <c r="J7" s="15"/>
+      <c r="K7" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="15" t="s">
         <v>23</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="D8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>36</v>
+        <v>32</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3" t="s">
-        <v>25</v>
+      <c r="J8" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="F9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="13"/>
+      <c r="G9" s="6"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3" t="s">
-        <v>24</v>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>20</v>
+      <c r="B10" s="15" t="s">
+        <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="3" t="s">
         <v>26</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>25</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="K10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>25</v>
+      <c r="L10" s="15" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="21" x14ac:dyDescent="0.35">
@@ -901,14 +906,14 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="3" t="s">
-        <v>26</v>
+      <c r="E11" s="15" t="s">
+        <v>25</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
+      <c r="J11" s="15"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>

</xml_diff>